<commit_message>
Encoding reports error solution
</commit_message>
<xml_diff>
--- a/output/excel/porownanie_krajow.xlsx
+++ b/output/excel/porownanie_krajow.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,24 +473,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1988</v>
+        <v>1991</v>
       </c>
       <c r="E2" t="n">
-        <v>11618005</v>
+        <v>56758521</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -498,1791 +498,1704 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1989</v>
+        <v>1992</v>
       </c>
       <c r="E3" t="n">
-        <v>11868877</v>
+        <v>56797087</v>
       </c>
       <c r="F3" t="n">
-        <v>250872</v>
+        <v>38566</v>
       </c>
       <c r="G3" t="n">
-        <v>2.15933802748407</v>
+        <v>0.06794750694789631</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1990</v>
+        <v>1993</v>
       </c>
       <c r="E4" t="n">
-        <v>12412308</v>
+        <v>56831821</v>
       </c>
       <c r="F4" t="n">
-        <v>543431</v>
+        <v>34734</v>
       </c>
       <c r="G4" t="n">
-        <v>4.578621886468293</v>
+        <v>0.06115454477444437</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1991</v>
+        <v>1994</v>
       </c>
       <c r="E5" t="n">
-        <v>13299017</v>
+        <v>56843400</v>
       </c>
       <c r="F5" t="n">
-        <v>886709</v>
+        <v>11579</v>
       </c>
       <c r="G5" t="n">
-        <v>7.143788246311655</v>
+        <v>0.0203741491936249</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1992</v>
+        <v>1995</v>
       </c>
       <c r="E6" t="n">
-        <v>14485546</v>
+        <v>56844303</v>
       </c>
       <c r="F6" t="n">
-        <v>1186529</v>
+        <v>903</v>
       </c>
       <c r="G6" t="n">
-        <v>8.921930094532549</v>
+        <v>0.001588574926913999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1993</v>
+        <v>1996</v>
       </c>
       <c r="E7" t="n">
-        <v>15816603</v>
+        <v>56860281</v>
       </c>
       <c r="F7" t="n">
-        <v>1331057</v>
+        <v>15978</v>
       </c>
       <c r="G7" t="n">
-        <v>9.188863160560178</v>
+        <v>0.02810835766602349</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1994</v>
+        <v>1997</v>
       </c>
       <c r="E8" t="n">
-        <v>17075727</v>
+        <v>56890372</v>
       </c>
       <c r="F8" t="n">
-        <v>1259124</v>
+        <v>30091</v>
       </c>
       <c r="G8" t="n">
-        <v>7.960773877930682</v>
+        <v>0.05292094845610329</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1995</v>
+        <v>1998</v>
       </c>
       <c r="E9" t="n">
-        <v>18110657</v>
+        <v>56906744</v>
       </c>
       <c r="F9" t="n">
-        <v>1034930</v>
+        <v>16372</v>
       </c>
       <c r="G9" t="n">
-        <v>6.060825404388348</v>
+        <v>0.02877815599449107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1996</v>
+        <v>1999</v>
       </c>
       <c r="E10" t="n">
-        <v>18853437</v>
+        <v>56916317</v>
       </c>
       <c r="F10" t="n">
-        <v>742780</v>
+        <v>9573</v>
       </c>
       <c r="G10" t="n">
-        <v>4.101342099295469</v>
+        <v>0.0168222592387357</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1997</v>
+        <v>2000</v>
       </c>
       <c r="E11" t="n">
-        <v>19357126</v>
+        <v>56942108</v>
       </c>
       <c r="F11" t="n">
-        <v>503689</v>
+        <v>25791</v>
       </c>
       <c r="G11" t="n">
-        <v>2.671603061022765</v>
+        <v>0.04531389478346082</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1998</v>
+        <v>2001</v>
       </c>
       <c r="E12" t="n">
-        <v>19737765</v>
+        <v>56974100</v>
       </c>
       <c r="F12" t="n">
-        <v>380639</v>
+        <v>31992</v>
       </c>
       <c r="G12" t="n">
-        <v>1.966402450446414</v>
+        <v>0.05618337838844134</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1999</v>
+        <v>2002</v>
       </c>
       <c r="E13" t="n">
-        <v>20170844</v>
+        <v>57059007</v>
       </c>
       <c r="F13" t="n">
-        <v>433079</v>
+        <v>84907</v>
       </c>
       <c r="G13" t="n">
-        <v>2.19416433420907</v>
+        <v>0.1490273650658791</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2000</v>
+        <v>2003</v>
       </c>
       <c r="E14" t="n">
-        <v>20779953</v>
+        <v>57313203</v>
       </c>
       <c r="F14" t="n">
-        <v>609109</v>
+        <v>254196</v>
       </c>
       <c r="G14" t="n">
-        <v>3.019749694162521</v>
+        <v>0.4454967118513009</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2001</v>
+        <v>2004</v>
       </c>
       <c r="E15" t="n">
-        <v>21606988</v>
+        <v>57685327</v>
       </c>
       <c r="F15" t="n">
-        <v>827035</v>
+        <v>372124</v>
       </c>
       <c r="G15" t="n">
-        <v>3.979965690971476</v>
+        <v>0.6492814578867634</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2002</v>
+        <v>2005</v>
       </c>
       <c r="E16" t="n">
-        <v>22600770</v>
+        <v>57969484</v>
       </c>
       <c r="F16" t="n">
-        <v>993782</v>
+        <v>284157</v>
       </c>
       <c r="G16" t="n">
-        <v>4.599354616201023</v>
+        <v>0.4925984037500664</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="E17" t="n">
-        <v>23680871</v>
+        <v>58143979</v>
       </c>
       <c r="F17" t="n">
-        <v>1080101</v>
+        <v>174495</v>
       </c>
       <c r="G17" t="n">
-        <v>4.779045138727578</v>
+        <v>0.3010118220131197</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="E18" t="n">
-        <v>24726684</v>
+        <v>58438310</v>
       </c>
       <c r="F18" t="n">
-        <v>1045813</v>
+        <v>294331</v>
       </c>
       <c r="G18" t="n">
-        <v>4.416277593843576</v>
+        <v>0.5062106258672205</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="E19" t="n">
-        <v>25654277</v>
+        <v>58826731</v>
       </c>
       <c r="F19" t="n">
-        <v>927593</v>
+        <v>388421</v>
       </c>
       <c r="G19" t="n">
-        <v>3.751384536640656</v>
+        <v>0.6646684341145459</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="E20" t="n">
-        <v>26433049</v>
+        <v>59095365</v>
       </c>
       <c r="F20" t="n">
-        <v>778772</v>
+        <v>268634</v>
       </c>
       <c r="G20" t="n">
-        <v>3.035641971122405</v>
+        <v>0.4566529457501245</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="E21" t="n">
-        <v>27100536</v>
+        <v>59277417</v>
       </c>
       <c r="F21" t="n">
-        <v>667487</v>
+        <v>182052</v>
       </c>
       <c r="G21" t="n">
-        <v>2.525198663234041</v>
+        <v>0.3080647695466565</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2008</v>
+        <v>1991</v>
       </c>
       <c r="E22" t="n">
-        <v>27722276</v>
-      </c>
-      <c r="F22" t="n">
-        <v>621740</v>
-      </c>
-      <c r="G22" t="n">
-        <v>2.294198166412653</v>
-      </c>
+        <v>8288735</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="E23" t="n">
-        <v>24190638</v>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+        <v>8566770</v>
+      </c>
+      <c r="F23" t="n">
+        <v>278035</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3.354371927682576</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1989</v>
+        <v>1993</v>
       </c>
       <c r="E24" t="n">
-        <v>24669512</v>
+        <v>8860287</v>
       </c>
       <c r="F24" t="n">
-        <v>478874</v>
+        <v>293517</v>
       </c>
       <c r="G24" t="n">
-        <v>1.97958400270386</v>
+        <v>3.426227154458439</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="E25" t="n">
-        <v>25134362</v>
+        <v>9168312</v>
       </c>
       <c r="F25" t="n">
-        <v>464850</v>
+        <v>308025</v>
       </c>
       <c r="G25" t="n">
-        <v>1.884309669360307</v>
+        <v>3.476467523004612</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="E26" t="n">
-        <v>25593376</v>
+        <v>9490288</v>
       </c>
       <c r="F26" t="n">
-        <v>459014</v>
+        <v>321976</v>
       </c>
       <c r="G26" t="n">
-        <v>1.826240904782073</v>
+        <v>3.511835112068606</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="E27" t="n">
-        <v>26020302</v>
+        <v>9826598</v>
       </c>
       <c r="F27" t="n">
-        <v>426926</v>
+        <v>336310</v>
       </c>
       <c r="G27" t="n">
-        <v>1.668111311301801</v>
+        <v>3.543728072319818</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="E28" t="n">
-        <v>26428552</v>
+        <v>10178201</v>
       </c>
       <c r="F28" t="n">
-        <v>408250</v>
+        <v>351603</v>
       </c>
       <c r="G28" t="n">
-        <v>1.568967185699832</v>
+        <v>3.578074527929198</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="E29" t="n">
-        <v>26841234</v>
+        <v>10545716</v>
       </c>
       <c r="F29" t="n">
-        <v>412682</v>
+        <v>367515</v>
       </c>
       <c r="G29" t="n">
-        <v>1.561500607373412</v>
+        <v>3.610805092176905</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1995</v>
+        <v>1999</v>
       </c>
       <c r="E30" t="n">
-        <v>27247899</v>
+        <v>10929918</v>
       </c>
       <c r="F30" t="n">
-        <v>406665</v>
+        <v>384202</v>
       </c>
       <c r="G30" t="n">
-        <v>1.515075648161335</v>
+        <v>3.643204501240116</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="E31" t="n">
-        <v>27660288</v>
+        <v>11331557</v>
       </c>
       <c r="F31" t="n">
-        <v>412389</v>
+        <v>401639</v>
       </c>
       <c r="G31" t="n">
-        <v>1.513470818428964</v>
+        <v>3.67467532693293</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1997</v>
+        <v>2001</v>
       </c>
       <c r="E32" t="n">
-        <v>28081620</v>
+        <v>11751365</v>
       </c>
       <c r="F32" t="n">
-        <v>421332</v>
+        <v>419808</v>
       </c>
       <c r="G32" t="n">
-        <v>1.523237935917376</v>
+        <v>3.704768903337818</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="E33" t="n">
-        <v>28504847</v>
+        <v>12189983</v>
       </c>
       <c r="F33" t="n">
-        <v>423227</v>
+        <v>438618</v>
       </c>
       <c r="G33" t="n">
-        <v>1.507131711062248</v>
+        <v>3.732485545296238</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="E34" t="n">
-        <v>28948606</v>
+        <v>12647984</v>
       </c>
       <c r="F34" t="n">
-        <v>443759</v>
+        <v>458001</v>
       </c>
       <c r="G34" t="n">
-        <v>1.556784360217756</v>
+        <v>3.757191457937226</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="E35" t="n">
-        <v>29393029</v>
+        <v>13125916</v>
       </c>
       <c r="F35" t="n">
-        <v>444423</v>
+        <v>477932</v>
       </c>
       <c r="G35" t="n">
-        <v>1.535213819967707</v>
+        <v>3.778720782695477</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="E36" t="n">
-        <v>29820335</v>
+        <v>13624467</v>
       </c>
       <c r="F36" t="n">
-        <v>427306</v>
+        <v>498551</v>
       </c>
       <c r="G36" t="n">
-        <v>1.453766469593853</v>
+        <v>3.798218730029967</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="E37" t="n">
-        <v>30250175</v>
+        <v>14143971</v>
       </c>
       <c r="F37" t="n">
-        <v>429840</v>
+        <v>519504</v>
       </c>
       <c r="G37" t="n">
-        <v>1.441432498997752</v>
+        <v>3.81302255713929</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2003</v>
+        <v>2007</v>
       </c>
       <c r="E38" t="n">
-        <v>30697311</v>
+        <v>14685399</v>
       </c>
       <c r="F38" t="n">
-        <v>447136</v>
+        <v>541428</v>
       </c>
       <c r="G38" t="n">
-        <v>1.478126986042239</v>
+        <v>3.82797730566613</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="E39" t="n">
-        <v>31189626</v>
+        <v>15250908</v>
       </c>
       <c r="F39" t="n">
-        <v>492315</v>
+        <v>565509</v>
       </c>
       <c r="G39" t="n">
-        <v>1.603772395569103</v>
+        <v>3.850824890763938</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2005</v>
+        <v>2009</v>
       </c>
       <c r="E40" t="n">
-        <v>31746604</v>
+        <v>15843133</v>
       </c>
       <c r="F40" t="n">
-        <v>556978</v>
+        <v>592225</v>
       </c>
       <c r="G40" t="n">
-        <v>1.785779669175902</v>
+        <v>3.883211412723764</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Niger</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="E41" t="n">
-        <v>32375210</v>
+        <v>16464025</v>
       </c>
       <c r="F41" t="n">
-        <v>628606</v>
+        <v>620892</v>
       </c>
       <c r="G41" t="n">
-        <v>1.980073207200372</v>
+        <v>3.918997587156525</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2007</v>
+        <v>1991</v>
       </c>
       <c r="E42" t="n">
-        <v>33066727</v>
-      </c>
-      <c r="F42" t="n">
-        <v>691517</v>
-      </c>
-      <c r="G42" t="n">
-        <v>2.135945990775046</v>
-      </c>
+        <v>320780</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Small states</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SST</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>2008</v>
+        <v>1992</v>
       </c>
       <c r="E43" t="n">
-        <v>33798838</v>
+        <v>329995</v>
       </c>
       <c r="F43" t="n">
-        <v>732111</v>
+        <v>9215</v>
       </c>
       <c r="G43" t="n">
-        <v>2.214041323170579</v>
+        <v>2.872685329509328</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1988</v>
+        <v>1993</v>
       </c>
       <c r="E44" t="n">
-        <v>1084281155</v>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
+        <v>339504</v>
+      </c>
+      <c r="F44" t="n">
+        <v>9509</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2.881558811497142</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1989</v>
+        <v>1994</v>
       </c>
       <c r="E45" t="n">
-        <v>1108702403</v>
+        <v>349281</v>
       </c>
       <c r="F45" t="n">
-        <v>24421248</v>
+        <v>9777</v>
       </c>
       <c r="G45" t="n">
-        <v>2.252298482490911</v>
+        <v>2.879789339742689</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1990</v>
+        <v>1995</v>
       </c>
       <c r="E46" t="n">
-        <v>1133495196</v>
+        <v>359281</v>
       </c>
       <c r="F46" t="n">
-        <v>24792793</v>
+        <v>10000</v>
       </c>
       <c r="G46" t="n">
-        <v>2.236199085788404</v>
+        <v>2.863024327117714</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1991</v>
+        <v>1996</v>
       </c>
       <c r="E47" t="n">
-        <v>1158655617</v>
+        <v>369523</v>
       </c>
       <c r="F47" t="n">
-        <v>25160421</v>
+        <v>10242</v>
       </c>
       <c r="G47" t="n">
-        <v>2.219720126630342</v>
+        <v>2.850693468343724</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1992</v>
+        <v>1997</v>
       </c>
       <c r="E48" t="n">
-        <v>1184133314</v>
+        <v>379999</v>
       </c>
       <c r="F48" t="n">
-        <v>25477697</v>
+        <v>10476</v>
       </c>
       <c r="G48" t="n">
-        <v>2.198901608570036</v>
+        <v>2.83500621070949</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1993</v>
+        <v>1998</v>
       </c>
       <c r="E49" t="n">
-        <v>1209847786</v>
+        <v>390693</v>
       </c>
       <c r="F49" t="n">
-        <v>25714472</v>
+        <v>10694</v>
       </c>
       <c r="G49" t="n">
-        <v>2.171585892903938</v>
+        <v>2.814217932152463</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1994</v>
+        <v>1999</v>
       </c>
       <c r="E50" t="n">
-        <v>1235693869</v>
+        <v>401586</v>
       </c>
       <c r="F50" t="n">
-        <v>25846083</v>
+        <v>10893</v>
       </c>
       <c r="G50" t="n">
-        <v>2.136308657922359</v>
+        <v>2.788122643610191</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1995</v>
+        <v>2000</v>
       </c>
       <c r="E51" t="n">
-        <v>1261587756</v>
+        <v>412660</v>
       </c>
       <c r="F51" t="n">
-        <v>25893887</v>
+        <v>11074</v>
       </c>
       <c r="G51" t="n">
-        <v>2.095493685742311</v>
+        <v>2.757566249819465</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1996</v>
+        <v>2001</v>
       </c>
       <c r="E52" t="n">
-        <v>1287476190</v>
+        <v>423944</v>
       </c>
       <c r="F52" t="n">
-        <v>25888434</v>
+        <v>11284</v>
       </c>
       <c r="G52" t="n">
-        <v>2.052051779741593</v>
+        <v>2.734454514612517</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>1997</v>
+        <v>2002</v>
       </c>
       <c r="E53" t="n">
-        <v>1313346377</v>
+        <v>435432</v>
       </c>
       <c r="F53" t="n">
-        <v>25870187</v>
+        <v>11488</v>
       </c>
       <c r="G53" t="n">
-        <v>2.00937207234877</v>
+        <v>2.70979185930218</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>1998</v>
+        <v>2003</v>
       </c>
       <c r="E54" t="n">
-        <v>1339202708</v>
+        <v>447017</v>
       </c>
       <c r="F54" t="n">
-        <v>25856331</v>
+        <v>11585</v>
       </c>
       <c r="G54" t="n">
-        <v>1.968736614560296</v>
+        <v>2.660576163442285</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>1999</v>
+        <v>2004</v>
       </c>
       <c r="E55" t="n">
-        <v>1365067928</v>
+        <v>458539</v>
       </c>
       <c r="F55" t="n">
-        <v>25865220</v>
+        <v>11522</v>
       </c>
       <c r="G55" t="n">
-        <v>1.931389463707678</v>
+        <v>2.577530608455603</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="E56" t="n">
-        <v>1390946064</v>
+        <v>469918</v>
       </c>
       <c r="F56" t="n">
-        <v>25878136</v>
+        <v>11379</v>
       </c>
       <c r="G56" t="n">
-        <v>1.895739799404317</v>
+        <v>2.481577357651155</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="E57" t="n">
-        <v>1416822959</v>
+        <v>481078</v>
       </c>
       <c r="F57" t="n">
-        <v>25876895</v>
+        <v>11160</v>
       </c>
       <c r="G57" t="n">
-        <v>1.860380906904813</v>
+        <v>2.374882426295644</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>2002</v>
+        <v>2007</v>
       </c>
       <c r="E58" t="n">
-        <v>1442644058</v>
+        <v>492132</v>
       </c>
       <c r="F58" t="n">
-        <v>25821099</v>
+        <v>11054</v>
       </c>
       <c r="G58" t="n">
-        <v>1.82246475016361</v>
+        <v>2.297756289000952</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="E59" t="n">
-        <v>1468324422</v>
+        <v>503360</v>
       </c>
       <c r="F59" t="n">
-        <v>25680364</v>
+        <v>11228</v>
       </c>
       <c r="G59" t="n">
-        <v>1.780090096208609</v>
+        <v>2.281501710923095</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="E60" t="n">
-        <v>1493757846</v>
+        <v>515181</v>
       </c>
       <c r="F60" t="n">
-        <v>25433424</v>
+        <v>11821</v>
       </c>
       <c r="G60" t="n">
-        <v>1.732139275144462</v>
+        <v>2.348418626827709</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>South Asia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="E61" t="n">
-        <v>1518861552</v>
+        <v>527861</v>
       </c>
       <c r="F61" t="n">
-        <v>25103706</v>
+        <v>12680</v>
       </c>
       <c r="G61" t="n">
-        <v>1.680574001149049</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>South Asia</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>2006</v>
-      </c>
-      <c r="E62" t="n">
-        <v>1543610696</v>
-      </c>
-      <c r="F62" t="n">
-        <v>24749144</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1.629453584325113</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>South Asia</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>2007</v>
-      </c>
-      <c r="E63" t="n">
-        <v>1568003159</v>
-      </c>
-      <c r="F63" t="n">
-        <v>24392463</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1.580221169962659</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>South Asia</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>2008</v>
-      </c>
-      <c r="E64" t="n">
-        <v>1592010819</v>
-      </c>
-      <c r="F64" t="n">
-        <v>24007660</v>
-      </c>
-      <c r="G64" t="n">
-        <v>1.531097680652049</v>
+        <v>2.461270893142409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>